<commit_message>
se agrega brecha enge y sin enge vs eeuu
</commit_message>
<xml_diff>
--- a/results/enge/brecha_enge_eeuu.xlsx
+++ b/results/enge/brecha_enge_eeuu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,24 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>brecha_productividad_sin_enge_tot_level</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>brecha_productividad_eeuu_arg</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>brecha_enge_eeuu</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>brecha_sin_enge_eeuu</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -466,10 +476,16 @@
         <v>2.742958567227117</v>
       </c>
       <c r="D2" t="n">
+        <v>0.7217866279342013</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.199</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.5458487548781963</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.143635538958906</v>
       </c>
     </row>
     <row r="3">
@@ -483,10 +499,16 @@
         <v>2.775950752599583</v>
       </c>
       <c r="D3" t="n">
+        <v>0.7061347470885972</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.219</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.6079332148193086</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1546435096124028</v>
       </c>
     </row>
     <row r="4">
@@ -500,10 +522,16 @@
         <v>2.58316985514918</v>
       </c>
       <c r="D4" t="n">
+        <v>0.7205939142286747</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.215</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.5553815188570738</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1549276915591651</v>
       </c>
     </row>
     <row r="5">
@@ -517,10 +545,16 @@
         <v>2.528455911252311</v>
       </c>
       <c r="D5" t="n">
+        <v>0.7274295185965005</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.228</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.5764879477655269</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1658539302400021</v>
       </c>
     </row>
     <row r="6">
@@ -534,10 +568,16 @@
         <v>2.585850152814536</v>
       </c>
       <c r="D6" t="n">
+        <v>0.7158631339776839</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.227</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.5869879846888997</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1625009314129342</v>
       </c>
     </row>
     <row r="7">
@@ -551,10 +591,16 @@
         <v>2.81090475724961</v>
       </c>
       <c r="D7" t="n">
+        <v>0.6964979768282287</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.209</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.5874790942651685</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1455680771570998</v>
       </c>
     </row>
     <row r="8">
@@ -568,10 +614,16 @@
         <v>2.820121541755504</v>
       </c>
       <c r="D8" t="n">
+        <v>0.7044691905273722</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.19</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.5358230929335458</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1338491462002007</v>
       </c>
     </row>
     <row r="9">
@@ -585,10 +637,16 @@
         <v>3.118346890992276</v>
       </c>
       <c r="D9" t="n">
+        <v>0.6572341654741737</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.181</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.564420787269602</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1189593839508254</v>
       </c>
     </row>
     <row r="10">
@@ -602,10 +660,16 @@
         <v>3.334211116972581</v>
       </c>
       <c r="D10" t="n">
+        <v>0.640122874364606</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.165</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.5501448343004759</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.10562027427016</v>
       </c>
     </row>
     <row r="11">
@@ -619,10 +683,16 @@
         <v>4.577053210441607</v>
       </c>
       <c r="D11" t="n">
+        <v>0.4664758337295752</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.135</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.6179021834096169</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.06297423755349266</v>
       </c>
     </row>
     <row r="12">
@@ -636,10 +706,16 @@
         <v>4.702982444247029</v>
       </c>
       <c r="D12" t="n">
+        <v>0.5188359339706339</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.129</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.6066847353078667</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.06692983548221178</v>
       </c>
     </row>
     <row r="13">
@@ -653,10 +729,16 @@
         <v>4.770290179674261</v>
       </c>
       <c r="D13" t="n">
+        <v>0.4876241351803389</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.135</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>0.6439891742560253</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.06582925824934575</v>
       </c>
     </row>
     <row r="14">
@@ -670,10 +752,16 @@
         <v>4.869433182748889</v>
       </c>
       <c r="D14" t="n">
+        <v>0.4848687707668133</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.128</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>0.6232874473918578</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0620632026581521</v>
       </c>
     </row>
     <row r="15">
@@ -687,10 +775,16 @@
         <v>4.775069496795604</v>
       </c>
       <c r="D15" t="n">
+        <v>0.4933955560261969</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.131</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>0.6255341040802241</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0646348178394318</v>
       </c>
     </row>
     <row r="16">
@@ -704,10 +798,16 @@
         <v>4.712520851014697</v>
       </c>
       <c r="D16" t="n">
+        <v>0.4607912212026656</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.136</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>0.6409028357379989</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.06266760608356252</v>
       </c>
     </row>
     <row r="17">
@@ -721,10 +821,16 @@
         <v>4.783464410961465</v>
       </c>
       <c r="D17" t="n">
+        <v>0.4512128566514683</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.136</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>0.6505511598907593</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0613649485045997</v>
       </c>
     </row>
     <row r="18">
@@ -738,10 +844,16 @@
         <v>4.724046406397718</v>
       </c>
       <c r="D18" t="n">
+        <v>0.4811258478933602</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.123</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>0.5810577079869194</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.05917847929088331</v>
       </c>
     </row>
     <row r="19">
@@ -755,10 +867,16 @@
         <v>4.096842967456881</v>
       </c>
       <c r="D19" t="n">
+        <v>0.5071842261070042</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.136</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>0.5571706435741359</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.06897705475055257</v>
       </c>
     </row>
     <row r="20">
@@ -772,10 +890,16 @@
         <v>4.123156790721839</v>
       </c>
       <c r="D20" t="n">
+        <v>0.5093578642283374</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.137</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>0.5648724803288918</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.06978202739928221</v>
       </c>
     </row>
     <row r="21">
@@ -789,10 +913,16 @@
         <v>4.406473209877951</v>
       </c>
       <c r="D21" t="n">
+        <v>0.473622428045198</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.127</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>0.5596220976544998</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.06015004836174015</v>
       </c>
     </row>
     <row r="22">
@@ -806,10 +936,16 @@
         <v>4.272122040764494</v>
       </c>
       <c r="D22" t="n">
+        <v>0.4723300233404075</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.128</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>0.5468316212178552</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.06045824298757217</v>
       </c>
     </row>
     <row r="23">
@@ -823,10 +959,16 @@
         <v>4.45713109920513</v>
       </c>
       <c r="D23" t="n">
+        <v>0.4421653496897042</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.121</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>0.5393128630038206</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.05350200731245421</v>
       </c>
     </row>
     <row r="24">
@@ -840,10 +982,16 @@
         <v>4.382485073009095</v>
       </c>
       <c r="D24" t="n">
+        <v>0.4454741915504722</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.128</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>0.5609580893451641</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.05702069651846044</v>
       </c>
     </row>
     <row r="25">
@@ -857,10 +1005,16 @@
         <v>4.601624364097165</v>
       </c>
       <c r="D25" t="n">
+        <v>0.4774814540996213</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.118</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>0.5429916749634655</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.05634281158375531</v>
       </c>
     </row>
     <row r="26">
@@ -874,10 +1028,16 @@
         <v>5.041055587269802</v>
       </c>
       <c r="D26" t="n">
+        <v>0.4121049083080825</v>
+      </c>
+      <c r="E26" t="n">
         <v>0.115</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>0.5797213925360273</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.04739206445542949</v>
       </c>
     </row>
     <row r="27">
@@ -890,8 +1050,12 @@
       <c r="C27" t="n">
         <v>5.290909880903697</v>
       </c>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>0.3820579528613384</v>
+      </c>
       <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -903,8 +1067,12 @@
       <c r="C28" t="n">
         <v>5.26298298466751</v>
       </c>
-      <c r="D28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>0.4268772236080584</v>
+      </c>
       <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -916,8 +1084,12 @@
       <c r="C29" t="n">
         <v>4.185006780429243</v>
       </c>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>0.5274793916539007</v>
+      </c>
       <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
se agregan estimaciones de rotacion
</commit_message>
<xml_diff>
--- a/results/enge/brecha_enge_eeuu.xlsx
+++ b/results/enge/brecha_enge_eeuu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -999,22 +999,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C25" t="n">
-        <v>4.601624364097165</v>
+        <v>4.279618508306799</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4774814540996213</v>
+        <v>0.4665957380533359</v>
       </c>
       <c r="E25" t="n">
-        <v>0.118</v>
+        <v>0.124</v>
       </c>
       <c r="F25" t="n">
-        <v>0.5429916749634655</v>
+        <v>0.530672695030043</v>
       </c>
       <c r="G25" t="n">
-        <v>0.05634281158375531</v>
+        <v>0.05785787151861366</v>
       </c>
     </row>
     <row r="26">
@@ -1022,22 +1022,22 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C26" t="n">
-        <v>5.041055587269802</v>
+        <v>4.601624364097165</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4121049083080825</v>
+        <v>0.4774814540996213</v>
       </c>
       <c r="E26" t="n">
-        <v>0.115</v>
+        <v>0.118</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5797213925360273</v>
+        <v>0.5429916749634655</v>
       </c>
       <c r="G26" t="n">
-        <v>0.04739206445542949</v>
+        <v>0.05634281158375531</v>
       </c>
     </row>
     <row r="27">
@@ -1045,30 +1045,36 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C27" t="n">
-        <v>5.290909880903697</v>
+        <v>5.041055587269802</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3820579528613384</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+        <v>0.4121049083080825</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.115</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.5797213925360273</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.04739206445542949</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C28" t="n">
-        <v>5.26298298466751</v>
+        <v>5.290909880903697</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4268772236080584</v>
+        <v>0.3820579528613384</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -1079,17 +1085,34 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C29" t="n">
-        <v>4.185006780429243</v>
+        <v>5.26298298466751</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5274793916539007</v>
+        <v>0.4268772236080584</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2021</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4.185006780429243</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5274793916539007</v>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>